<commit_message>
xlsx generation fix; some other fixes
</commit_message>
<xml_diff>
--- a/backend/docs/ResultTable.xlsx
+++ b/backend/docs/ResultTable.xlsx
@@ -551,8 +551,8 @@
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="5.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="5" style="0" width="8.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="3" width="8.5"/>

</xml_diff>